<commit_message>
el genesis format fix
</commit_message>
<xml_diff>
--- a/el-genesis/checklist.xlsx
+++ b/el-genesis/checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/el-genesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC76F3C4-F48C-E145-8582-791E2F4ABA7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D292ECC-2EE4-9747-BB72-F49F3E525DC3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{65EF623E-CBD3-1249-935E-98838B76FCED}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="16340" xr2:uid="{65EF623E-CBD3-1249-935E-98838B76FCED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
   <si>
     <t>year</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>Divine Era: El Genesis</t>
+  </si>
+  <si>
+    <t>supplement</t>
   </si>
 </sst>
 </file>
@@ -483,7 +486,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -516,19 +519,19 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>1999</v>
+        <v>1996</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
         <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F2" t="s">
         <v>16</v>
@@ -536,19 +539,19 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>1996</v>
+        <v>1998</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F3" t="s">
         <v>16</v>
@@ -556,19 +559,19 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F4" t="s">
         <v>16</v>
@@ -576,22 +579,22 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>1997</v>
+        <v>1999</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -608,7 +611,7 @@
         <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -625,7 +628,7 @@
         <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -642,7 +645,7 @@
         <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>